<commit_message>
Added Invoices. Created 1 workflow to get Invoice path. Created empty workflow which will get text from invoice when completed.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/FrameworkTemplates/REFramework/VB/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndreiHandrau\Documents\GitHub\Digi_Extraction\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D06465-0780-4834-85A5-6D82C5FCA7C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10248" yWindow="17508" windowWidth="21252" windowHeight="9444" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -160,6 +160,15 @@
   </si>
   <si>
     <t>ProcessABCQueue</t>
+  </si>
+  <si>
+    <t>invoicePath</t>
+  </si>
+  <si>
+    <t>Data\Input\Invoices</t>
+  </si>
+  <si>
+    <t>regex</t>
   </si>
 </sst>
 </file>
@@ -537,16 +546,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -594,7 +603,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -604,7 +613,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="29">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -616,9 +625,20 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1623,12 +1643,12 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1665,7 +1685,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1676,7 +1696,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1790,7 +1810,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -2786,12 +2806,12 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.90625" customWidth="1"/>
+    <col min="2" max="2" width="30.08984375" customWidth="1"/>
+    <col min="3" max="3" width="60.36328125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Added a different way to get transaction item(Now all invoices' names and paths are stored in an array and TransactionItem is now array(TransactionNumber)) Created a workflow to move invoice depending on the path specified in argument. Created a workflow to check if the invoice belongs to Digi and sends it into folders according to this and whether or not it contains all necessary data to be extract(Not completed yet). Created a workflow to add transaction item data to a data table which will be used to populate the report workbook to be sent through email
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndreiHandrau\Documents\GitHub\Digi_Extraction\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D06465-0780-4834-85A5-6D82C5FCA7C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36168945-059B-4BFF-A077-D2F07E4C14AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -169,6 +169,15 @@
   </si>
   <si>
     <t>regex</t>
+  </si>
+  <si>
+    <t>regexCompany</t>
+  </si>
+  <si>
+    <t>RCS &amp; RDS</t>
+  </si>
+  <si>
+    <t>(?&lt;=C\.I\.F\.: RO\d{7}\W)((\w+\W)+);((?&lt;=C\.I\.F\.: RO)\d{7});((?&lt;=IBAN:\s)(\S{4}\s)+);((?&lt;=Data:\s).+);(?&lt;=plat.:\s)(\d{2,4}.)+;((?&lt;=Num.r factur.:\s)\d+);((?&lt;=achitat:\s)\d+(,|.)\d+)</t>
   </si>
 </sst>
 </file>
@@ -547,7 +556,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -638,8 +647,18 @@
       <c r="A9" t="s">
         <v>47</v>
       </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Put workflows in corresponding folders. Created Test Cases. Additional minor fixes and whole project got stitched together.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndreiHandrau\Documents\GitHub\Digi_Extraction\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36168945-059B-4BFF-A077-D2F07E4C14AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2731F023-FE28-43D6-9925-5A9AD90E3695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -178,6 +178,54 @@
   </si>
   <si>
     <t>(?&lt;=C\.I\.F\.: RO\d{7}\W)((\w+\W)+);((?&lt;=C\.I\.F\.: RO)\d{7});((?&lt;=IBAN:\s)(\S{4}\s)+);((?&lt;=Data:\s).+);(?&lt;=plat.:\s)(\d{2,4}.)+;((?&lt;=Num.r factur.:\s)\d+);((?&lt;=achitat:\s)\d+(,|.)\d+)</t>
+  </si>
+  <si>
+    <t>unknownFolder</t>
+  </si>
+  <si>
+    <t>Unknown_Invoices</t>
+  </si>
+  <si>
+    <t>incompleteFolder</t>
+  </si>
+  <si>
+    <t>Incomplete_Invoices</t>
+  </si>
+  <si>
+    <t>processedFolder</t>
+  </si>
+  <si>
+    <t>Processed_Invoices</t>
+  </si>
+  <si>
+    <t>successText</t>
+  </si>
+  <si>
+    <t>COMPLETED</t>
+  </si>
+  <si>
+    <t>incompleteText</t>
+  </si>
+  <si>
+    <t>INCOMPLETE</t>
+  </si>
+  <si>
+    <t>reportPath</t>
+  </si>
+  <si>
+    <t>Data\Output\OutputReport</t>
+  </si>
+  <si>
+    <t>emailReceiver</t>
+  </si>
+  <si>
+    <t>handrauandrei@gmail.com</t>
+  </si>
+  <si>
+    <t>emailSubject</t>
+  </si>
+  <si>
+    <t>Digi Extraction Output Report</t>
   </si>
 </sst>
 </file>
@@ -229,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -239,6 +287,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -642,45 +692,101 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" t="s">
-        <v>50</v>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" t="s">
+        <v>62</v>
       </c>
     </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
         <v>48</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="17" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1647,6 +1753,7 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
+    <row r="999" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>